<commit_message>
++ enabeld generating users
</commit_message>
<xml_diff>
--- a/data/特征工程.xlsx
+++ b/data/特征工程.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Documents/lwx-game-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/coding/PycharmProjects/lxw-game-data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C503EF6-D323-E84E-9889-5A1C6649F678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B52C47-B9F2-4749-83B4-50ED4C4DA197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17920" yWindow="500" windowWidth="17920" windowHeight="21900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表2" sheetId="2" r:id="rId1"/>
@@ -741,9 +741,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -754,6 +751,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1032,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="140" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1043,8 +1043,8 @@
     <col min="3" max="3" width="42.83203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="11" style="5"/>
     <col min="5" max="5" width="15" style="3" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="32.33203125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="32.33203125" style="7" customWidth="1"/>
     <col min="8" max="16384" width="11" style="5"/>
   </cols>
   <sheetData>
@@ -1064,10 +1064,10 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1087,7 +1087,7 @@
       <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1107,7 +1107,7 @@
       <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1127,7 +1127,7 @@
       <c r="E4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1147,10 +1147,10 @@
       <c r="E5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1170,7 +1170,7 @@
       <c r="E6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1188,12 +1188,12 @@
       <c r="E7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="10" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1208,15 +1208,15 @@
       <c r="E8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17">
-      <c r="A9" s="7"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="1" t="s">
         <v>48</v>
       </c>
@@ -1229,12 +1229,12 @@
       <c r="E9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17">
-      <c r="A10" s="7"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="1" t="s">
         <v>51</v>
       </c>
@@ -1247,12 +1247,12 @@
       <c r="E10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="34">
-      <c r="A11" s="7"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="1" t="s">
         <v>54</v>
       </c>
@@ -1265,12 +1265,12 @@
       <c r="E11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="10" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17">
-      <c r="A12" s="7"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="1" t="s">
         <v>59</v>
       </c>
@@ -1283,12 +1283,12 @@
       <c r="E12" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17">
-      <c r="A13" s="7"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="1" t="s">
         <v>62</v>
       </c>
@@ -1301,12 +1301,12 @@
       <c r="E13" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="34">
-      <c r="A14" s="7"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="1" t="s">
         <v>65</v>
       </c>
@@ -1319,12 +1319,12 @@
       <c r="E14" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="10" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="51">
-      <c r="A15" s="7"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="1" t="s">
         <v>70</v>
       </c>
@@ -1337,15 +1337,15 @@
       <c r="E15" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="7" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="17">
-      <c r="A16" s="7"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="1" t="s">
         <v>76</v>
       </c>
@@ -1358,12 +1358,12 @@
       <c r="E16" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="17">
-      <c r="A17" s="7"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="1" t="s">
         <v>79</v>
       </c>
@@ -1376,7 +1376,7 @@
       <c r="E17" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="10" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1396,12 +1396,12 @@
       <c r="E18" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="10" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="17">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="11" t="s">
         <v>90</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1416,12 +1416,12 @@
       <c r="E19" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="34">
-      <c r="A20" s="7"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="1" t="s">
         <v>95</v>
       </c>
@@ -1434,15 +1434,15 @@
       <c r="E20" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="7" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="17">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="11" t="s">
         <v>101</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1457,12 +1457,12 @@
       <c r="E21" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="10" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17">
-      <c r="A22" s="7"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="1" t="s">
         <v>106</v>
       </c>
@@ -1475,7 +1475,7 @@
       <c r="E22" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="10" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1487,7 +1487,7 @@
       <c r="E23" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="10" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1501,7 +1501,7 @@
       <c r="E24" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="10" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1512,10 +1512,10 @@
       <c r="E25" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="G25" s="7" t="s">
         <v>200</v>
       </c>
     </row>
@@ -1526,7 +1526,7 @@
       <c r="E26" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="9" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1540,10 +1540,10 @@
       <c r="E27" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="7" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1592,7 +1592,7 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="11" t="s">
         <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1609,7 +1609,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="7"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="1" t="s">
         <v>125</v>
       </c>
@@ -1624,7 +1624,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="7"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="1" t="s">
         <v>129</v>
       </c>
@@ -1639,7 +1639,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="7"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="1" t="s">
         <v>131</v>
       </c>
@@ -1654,7 +1654,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="7"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="1" t="s">
         <v>133</v>
       </c>
@@ -1669,7 +1669,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="7"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="1" t="s">
         <v>136</v>
       </c>
@@ -1684,7 +1684,7 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="11" t="s">
         <v>138</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1696,38 +1696,38 @@
       <c r="D8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="11" t="s">
         <v>142</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="11" t="s">
         <v>144</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1738,29 +1738,29 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="7"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="1" t="s">
         <v>147</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="7"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="1" t="s">
         <v>149</v>
       </c>
@@ -1775,7 +1775,7 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="7"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="1" t="s">
         <v>151</v>
       </c>
@@ -1790,7 +1790,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="11" t="s">
         <v>154</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1807,7 +1807,7 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="7"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="1" t="s">
         <v>159</v>
       </c>
@@ -1822,7 +1822,7 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="7"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="1" t="s">
         <v>161</v>
       </c>
@@ -1838,7 +1838,7 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="7"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="1" t="s">
         <v>163</v>
       </c>
@@ -1853,33 +1853,33 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="7"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="1" t="s">
         <v>165</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="11" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="7"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="1" t="s">
         <v>169</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="11" t="s">
         <v>171</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1891,12 +1891,12 @@
       <c r="D22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="7"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="1" t="s">
         <v>174</v>
       </c>
@@ -1906,10 +1906,10 @@
       <c r="D23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="7"/>
+      <c r="E23" s="11"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="7"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="1" t="s">
         <v>176</v>
       </c>
@@ -1919,25 +1919,25 @@
       <c r="D24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="7"/>
+      <c r="E24" s="11"/>
     </row>
     <row r="25" spans="1:6" ht="16" customHeight="1">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7" t="s">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="11" t="s">
         <v>179</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="7"/>
+      <c r="E25" s="11"/>
     </row>
     <row r="26" spans="1:6" ht="16" customHeight="1">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
       <c r="D26" s="1" t="s">
         <v>89</v>
       </c>
@@ -1946,7 +1946,7 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="7"/>
+      <c r="A27" s="11"/>
       <c r="B27" s="1" t="s">
         <v>180</v>
       </c>
@@ -1961,7 +1961,7 @@
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="7"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="1" t="s">
         <v>183</v>
       </c>
@@ -1976,7 +1976,7 @@
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="11" t="s">
         <v>185</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1993,7 +1993,7 @@
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="7"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="1" t="s">
         <v>188</v>
       </c>
@@ -2008,7 +2008,7 @@
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="7"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="1" t="s">
         <v>190</v>
       </c>
@@ -2023,7 +2023,7 @@
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="7"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="1" t="s">
         <v>192</v>
       </c>
@@ -2038,7 +2038,7 @@
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="7"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="1" t="s">
         <v>195</v>
       </c>
@@ -2053,7 +2053,7 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="7"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="1" t="s">
         <v>197</v>
       </c>
@@ -2069,23 +2069,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A15"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E20:E21"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C25:C26"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A15"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="A29:A34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A16" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>

</xml_diff>